<commit_message>
wirings & pinouts updates
</commit_message>
<xml_diff>
--- a/Fiesta_pcbs/ecu/pinout.xlsx
+++ b/Fiesta_pcbs/ecu/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/NO NAME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE3F0DCD-40C3-3B47-95A6-E4217EA0BD50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3831C1E8-17A1-4D38-AD23-52FA7B7D88BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="520" windowWidth="23260" windowHeight="15480" xr2:uid="{B46B32A5-789C-497D-8B7F-BCFECB5EAE68}"/>
+    <workbookView xWindow="1968" yWindow="588" windowWidth="14580" windowHeight="11400" xr2:uid="{B46B32A5-789C-497D-8B7F-BCFECB5EAE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
   <si>
     <t>glow plugs relay</t>
   </si>
@@ -57,9 +57,6 @@
     <t>heater lo</t>
   </si>
   <si>
-    <t>heated glass</t>
-  </si>
-  <si>
     <t>hall sign</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>turbo pressure</t>
   </si>
   <si>
-    <t>H glass button</t>
-  </si>
-  <si>
     <t>misc 1</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>misc 2</t>
   </si>
   <si>
-    <t>turbo</t>
-  </si>
-  <si>
     <t>throttle pos</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>FAN</t>
   </si>
   <si>
-    <t>idle</t>
-  </si>
-  <si>
     <t>+12V / ignition</t>
   </si>
   <si>
@@ -130,6 +118,24 @@
   </si>
   <si>
     <t>SCL</t>
+  </si>
+  <si>
+    <t>DPF start</t>
+  </si>
+  <si>
+    <t>DPF lamp</t>
+  </si>
+  <si>
+    <t>H window button</t>
+  </si>
+  <si>
+    <t>heated window</t>
+  </si>
+  <si>
+    <t>idle solenoid</t>
+  </si>
+  <si>
+    <t>turbo solenoid</t>
   </si>
 </sst>
 </file>
@@ -518,22 +524,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D01CF8-590D-4266-A736-D70CAC428B5B}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -544,13 +551,13 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1">
         <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G1">
         <v>79</v>
@@ -559,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -582,10 +589,10 @@
         <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -602,7 +609,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>81</v>
@@ -611,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -637,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -648,22 +655,22 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -674,13 +681,13 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6">
         <v>84</v>
@@ -689,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -715,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -726,7 +733,7 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>60</v>
@@ -741,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -752,7 +759,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <v>61</v>
@@ -767,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -793,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -810,7 +817,7 @@
         <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11">
         <v>89</v>
@@ -819,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -842,7 +849,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -852,6 +859,9 @@
       <c r="C13">
         <v>39</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E13">
         <v>65</v>
       </c>
@@ -862,12 +872,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -878,14 +888,17 @@
       <c r="E14">
         <v>66</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G14">
         <v>92</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -893,7 +906,7 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>67</v>
@@ -908,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -916,13 +929,13 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <v>94</v>
@@ -931,12 +944,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>43</v>
@@ -948,7 +961,7 @@
         <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G17">
         <v>95</v>
@@ -957,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -974,12 +987,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C19">
         <v>45</v>
@@ -991,16 +1004,16 @@
         <v>71</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G19">
         <v>97</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1023,12 +1036,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>47</v>
@@ -1049,12 +1062,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>48</v>
@@ -1072,18 +1085,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>49</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E23">
         <v>75</v>
@@ -1098,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1109,13 +1122,13 @@
         <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>76</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24">
         <v>102</v>
@@ -1124,33 +1137,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25">
         <v>77</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25">
         <v>103</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1178,6 +1191,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>